<commit_message>
push ya 3m ana yasser
</commit_message>
<xml_diff>
--- a/Integrated/ControlUnit.xlsx
+++ b/Integrated/ControlUnit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eng materials\6th semester\archtecture\Project\Integrated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Desktop\Integrated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77B54A2-410B-49DE-A7F5-0D8DFAA682CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B16ED61-83D1-411F-855D-6A85343EA696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9AB7CBDB-2903-4B43-8724-B8F9F56DAB9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9AB7CBDB-2903-4B43-8724-B8F9F56DAB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="74">
   <si>
     <t>Spselect</t>
   </si>
@@ -153,9 +153,6 @@
     <t>RET</t>
   </si>
   <si>
-    <t>Rest</t>
-  </si>
-  <si>
     <t>00</t>
   </si>
   <si>
@@ -255,13 +252,13 @@
     <t>Y</t>
   </si>
   <si>
-    <t>بيعمل jump صح بس بيدي error اول م تخلي ال jump flags ب 0</t>
-  </si>
-  <si>
-    <t>Error At line42 Ram</t>
-  </si>
-  <si>
-    <t>ال control unit بايظه و وبالتالي ال SP مش بيتحرك أصلا</t>
+    <t>REST</t>
+  </si>
+  <si>
+    <t>مش شغالة</t>
+  </si>
+  <si>
+    <t>because we never go back</t>
   </si>
 </sst>
 </file>
@@ -321,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="180"/>
@@ -340,6 +337,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,26 +756,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65687CC-1941-4D8F-87F6-9FFAC1C955AA}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16" width="4.88671875" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16" width="4.85546875" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="3.5703125" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="61.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="66.75" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>6</v>
@@ -795,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -804,10 +805,10 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
@@ -822,16 +823,16 @@
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -842,53 +843,53 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="3">
         <v>0</v>
       </c>
       <c r="R2" s="7"/>
       <c r="S2" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -899,51 +900,53 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="3">
         <v>0</v>
       </c>
       <c r="R3" s="7"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -954,51 +957,53 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="3">
         <v>0</v>
       </c>
       <c r="R4" s="7"/>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S4" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
@@ -1009,53 +1014,53 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="3">
         <v>0</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1066,53 +1071,53 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="3">
         <v>0</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1123,53 +1128,53 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="3">
         <v>0</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1180,53 +1185,55 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q8" s="3">
         <v>0</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1237,55 +1244,55 @@
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="3">
         <v>0</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1296,55 +1303,55 @@
         <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="3">
         <v>1</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1355,55 +1362,55 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="3">
         <v>1</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1414,55 +1421,55 @@
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q12" s="3">
         <v>0</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1473,53 +1480,53 @@
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q13" s="3">
         <v>1</v>
       </c>
       <c r="R13" s="7"/>
       <c r="S13" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
@@ -1530,53 +1537,53 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="3">
         <v>1</v>
       </c>
       <c r="R14" s="7"/>
       <c r="S14" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
@@ -1587,53 +1594,53 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q15" s="3">
         <v>1</v>
       </c>
       <c r="R15" s="7"/>
       <c r="S15" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
@@ -1644,53 +1651,54 @@
         <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="3">
         <v>0</v>
       </c>
       <c r="R16" s="7"/>
       <c r="S16" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="T16" s="2"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -1701,53 +1709,54 @@
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="3">
         <v>0</v>
       </c>
       <c r="R17" s="7"/>
-      <c r="S17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T17" s="2"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>27</v>
       </c>
@@ -1758,53 +1767,53 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q18" s="3">
         <v>0</v>
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
@@ -1815,53 +1824,53 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="O19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q19" s="3">
         <v>0</v>
       </c>
       <c r="R19" s="7"/>
-      <c r="S19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S19" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
@@ -1872,52 +1881,55 @@
         <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="3">
         <v>0</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>30</v>
       </c>
@@ -1928,52 +1940,55 @@
         <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="3">
         <v>0</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>31</v>
       </c>
@@ -1984,52 +1999,55 @@
         <v>7</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="3">
         <v>0</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>32</v>
       </c>
@@ -2040,56 +2058,54 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q23" s="3">
         <v>0</v>
       </c>
       <c r="R23" s="7"/>
       <c r="S23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>33</v>
       </c>
@@ -2100,56 +2116,53 @@
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q24" s="3">
         <v>0</v>
       </c>
       <c r="R24" s="7"/>
       <c r="S24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>34</v>
       </c>
@@ -2160,56 +2173,53 @@
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q25" s="3">
         <v>0</v>
       </c>
       <c r="R25" s="7"/>
       <c r="S25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>35</v>
       </c>
@@ -2220,56 +2230,53 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q26" s="3">
         <v>0</v>
       </c>
       <c r="R26" s="7"/>
       <c r="S26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -2280,50 +2287,50 @@
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q27" s="3">
         <v>0</v>
       </c>
       <c r="R27" s="7"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>37</v>
       </c>
@@ -2334,59 +2341,61 @@
         <v>14</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="O28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q28" s="3">
         <v>0</v>
       </c>
       <c r="R28" s="7"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="3">
-        <v>28</v>
-      </c>
-      <c r="C29" s="7">
-        <v>15</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2402,6 +2411,12 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="7"/>
+      <c r="S29" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="94" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T94" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2417,69 +2432,69 @@
       <selection activeCell="A2" sqref="A2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -2497,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>5</v>
@@ -2518,10 +2533,10 @@
         <v>8</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>